<commit_message>
Netzplan Übung FIAE D
</commit_message>
<xml_diff>
--- a/FIAED Übungen/Online_Shop.Projekt.FIAE_D.xlsx
+++ b/FIAED Übungen/Online_Shop.Projekt.FIAE_D.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="76">
   <si>
     <t xml:space="preserve">Beispiel: Funktionsorientierter Projektstrukturplan</t>
   </si>
@@ -199,6 +199,57 @@
   </si>
   <si>
     <t xml:space="preserve">1.3.1, 1.2.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Früheste</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anfangszeit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Endzeit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gesamtpuffer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Freier Puffer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Späteste</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FAZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FEZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FEZ_Vorgänger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FAZ + D</t>
   </si>
 </sst>
 </file>
@@ -273,7 +324,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -283,7 +334,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFBF00"/>
-        <bgColor rgb="FFFF9900"/>
+        <bgColor rgb="FFFF8000"/>
       </patternFill>
     </fill>
     <fill>
@@ -308,6 +359,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFE8E8E8"/>
         <bgColor rgb="FFEEEEEE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00A933"/>
+        <bgColor rgb="FF008000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF8000"/>
+        <bgColor rgb="FFFF6600"/>
       </patternFill>
     </fill>
   </fills>
@@ -403,7 +466,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="56">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -484,10 +547,18 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -496,6 +567,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -521,6 +596,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -540,7 +619,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -553,6 +632,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -562,6 +645,50 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -633,12 +760,12 @@
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFBF00"/>
-      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF8000"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666666"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF00A933"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
@@ -672,8 +799,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="5456880" y="479520"/>
-          <a:ext cx="5491800" cy="0"/>
+          <a:off x="5462280" y="479520"/>
+          <a:ext cx="5500800" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -714,7 +841,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5457600" y="488160"/>
+          <a:off x="5462640" y="488160"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -755,7 +882,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5456880" y="488160"/>
+          <a:off x="5461920" y="488160"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -797,7 +924,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5463360" y="1125360"/>
+          <a:off x="5469840" y="1125360"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -839,7 +966,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5463360" y="1612800"/>
+          <a:off x="5469840" y="1612800"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -881,7 +1008,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5463360" y="2099880"/>
+          <a:off x="5469840" y="2099880"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -923,7 +1050,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5463360" y="2587320"/>
+          <a:off x="5469840" y="2587320"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -965,7 +1092,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8200800" y="324720"/>
+          <a:off x="8210880" y="324720"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1007,7 +1134,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8200800" y="487440"/>
+          <a:off x="8210880" y="487440"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1049,7 +1176,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8200800" y="1125360"/>
+          <a:off x="8210880" y="1125360"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1091,7 +1218,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8200800" y="1612800"/>
+          <a:off x="8210880" y="1612800"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1133,7 +1260,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8200800" y="2587320"/>
+          <a:off x="8210880" y="2587320"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1175,7 +1302,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8200800" y="3074400"/>
+          <a:off x="8210880" y="3074400"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1217,7 +1344,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8200800" y="4048920"/>
+          <a:off x="8210880" y="4048920"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1259,7 +1386,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8200800" y="5023440"/>
+          <a:off x="8210880" y="5023440"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1301,7 +1428,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10938600" y="487440"/>
+          <a:off x="10952640" y="487440"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1343,7 +1470,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10938600" y="1125360"/>
+          <a:off x="10952640" y="1125360"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1385,7 +1512,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10938600" y="1612800"/>
+          <a:off x="10952640" y="1612800"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1427,7 +1554,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10938600" y="2099880"/>
+          <a:off x="10952640" y="2099880"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1469,7 +1596,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8199360" y="3557520"/>
+          <a:off x="8208360" y="3557520"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1511,7 +1638,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8199360" y="4533480"/>
+          <a:off x="8208360" y="4533480"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1553,7 +1680,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8199360" y="2093760"/>
+          <a:off x="8208360" y="2093760"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1585,13 +1712,13 @@
       <xdr:col>14</xdr:col>
       <xdr:colOff>10080</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>154080</xdr:rowOff>
+      <xdr:rowOff>154440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>4680</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>160200</xdr:rowOff>
+      <xdr:rowOff>160560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1600,7 +1727,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="7154280" y="478800"/>
+          <a:off x="7287120" y="479160"/>
           <a:ext cx="535680" cy="6120"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1625,15 +1752,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>267840</xdr:colOff>
+      <xdr:colOff>268560</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>160200</xdr:rowOff>
+      <xdr:rowOff>160560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>267840</xdr:colOff>
+      <xdr:colOff>268560</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>3240</xdr:rowOff>
+      <xdr:rowOff>3600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1642,7 +1769,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="8493840" y="484920"/>
+          <a:off x="8627040" y="485280"/>
           <a:ext cx="541080" cy="5400"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1669,13 +1796,13 @@
       <xdr:col>14</xdr:col>
       <xdr:colOff>255240</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>18000</xdr:rowOff>
+      <xdr:rowOff>18720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>3240</xdr:colOff>
+      <xdr:colOff>3600</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>18000</xdr:rowOff>
+      <xdr:rowOff>18720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1684,8 +1811,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7399080" y="505080"/>
-          <a:ext cx="18360" cy="1950840"/>
+          <a:off x="7532280" y="505800"/>
+          <a:ext cx="18720" cy="1950840"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1709,15 +1836,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>11880</xdr:colOff>
+      <xdr:colOff>12600</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>159480</xdr:rowOff>
+      <xdr:rowOff>159840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>264240</xdr:colOff>
+      <xdr:colOff>264960</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>159480</xdr:rowOff>
+      <xdr:rowOff>159840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1726,7 +1853,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="7426080" y="2435040"/>
+          <a:off x="7559640" y="2435400"/>
           <a:ext cx="252360" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1753,13 +1880,13 @@
       <xdr:col>24</xdr:col>
       <xdr:colOff>5040</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>154080</xdr:rowOff>
+      <xdr:rowOff>154440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>30</xdr:col>
-      <xdr:colOff>244440</xdr:colOff>
+      <xdr:colOff>244800</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>159480</xdr:rowOff>
+      <xdr:rowOff>159840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1768,7 +1895,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9854280" y="478800"/>
+          <a:off x="9987120" y="479160"/>
           <a:ext cx="1862640" cy="5400"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1793,15 +1920,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>267480</xdr:colOff>
+      <xdr:colOff>268200</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>160200</xdr:rowOff>
+      <xdr:rowOff>160560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>267480</xdr:colOff>
+      <xdr:colOff>268200</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>2520</xdr:rowOff>
+      <xdr:rowOff>2880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1810,7 +1937,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="8493480" y="2435760"/>
+          <a:off x="8626680" y="2436120"/>
           <a:ext cx="541080" cy="5040"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1835,15 +1962,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>265680</xdr:colOff>
+      <xdr:colOff>266040</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>160200</xdr:rowOff>
+      <xdr:rowOff>160560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>260280</xdr:colOff>
+      <xdr:colOff>260640</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>2520</xdr:rowOff>
+      <xdr:rowOff>2880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1852,7 +1979,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="9844560" y="2435760"/>
+          <a:off x="9977400" y="2436120"/>
           <a:ext cx="535680" cy="5040"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1879,13 +2006,13 @@
       <xdr:col>19</xdr:col>
       <xdr:colOff>257040</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>158040</xdr:rowOff>
+      <xdr:rowOff>158400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>257040</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>2520</xdr:rowOff>
+      <xdr:rowOff>2880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1894,7 +2021,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8753760" y="482760"/>
+          <a:off x="8886600" y="483120"/>
           <a:ext cx="0" cy="982440"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1919,15 +2046,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>253440</xdr:colOff>
+      <xdr:colOff>253800</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>155160</xdr:rowOff>
+      <xdr:rowOff>155520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>258120</xdr:colOff>
+      <xdr:colOff>258840</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>159120</xdr:rowOff>
+      <xdr:rowOff>159480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1936,7 +2063,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="8749800" y="1455120"/>
+          <a:off x="8883000" y="1455480"/>
           <a:ext cx="275400" cy="3960"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1961,7 +2088,7 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>257760</xdr:colOff>
+      <xdr:colOff>258120</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>155520</xdr:rowOff>
     </xdr:from>
@@ -1978,7 +2105,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9836640" y="1455840"/>
+          <a:off x="9969480" y="1455840"/>
           <a:ext cx="565920" cy="7200"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2020,7 +2147,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12544920" y="480240"/>
+          <a:off x="12677760" y="480240"/>
           <a:ext cx="560520" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2051,7 +2178,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>3240</xdr:colOff>
+      <xdr:colOff>3600</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>156600</xdr:rowOff>
     </xdr:to>
@@ -2062,7 +2189,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="10113120" y="1926720"/>
+          <a:off x="10245960" y="1926720"/>
           <a:ext cx="10080" cy="505440"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2087,15 +2214,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>264600</xdr:colOff>
+      <xdr:colOff>264960</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>155520</xdr:rowOff>
+      <xdr:rowOff>155880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
-      <xdr:colOff>257400</xdr:colOff>
+      <xdr:colOff>257760</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>160200</xdr:rowOff>
+      <xdr:rowOff>160560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2104,7 +2231,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="10113480" y="1943280"/>
+          <a:off x="10246680" y="1943640"/>
           <a:ext cx="1345320" cy="4680"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2129,15 +2256,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>29</xdr:col>
-      <xdr:colOff>263520</xdr:colOff>
+      <xdr:colOff>263880</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>146520</xdr:rowOff>
+      <xdr:rowOff>146880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
-      <xdr:colOff>264600</xdr:colOff>
+      <xdr:colOff>264960</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>25560</xdr:rowOff>
+      <xdr:rowOff>25920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2146,7 +2273,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="11464920" y="471240"/>
+          <a:off x="11598120" y="471600"/>
           <a:ext cx="1080" cy="1504440"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2177,7 +2304,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>30</xdr:col>
-      <xdr:colOff>9000</xdr:colOff>
+      <xdr:colOff>9360</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -2188,7 +2315,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11203560" y="1463040"/>
+          <a:off x="11336400" y="1463040"/>
           <a:ext cx="277920" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2213,7 +2340,7 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>39</xdr:col>
-      <xdr:colOff>10440</xdr:colOff>
+      <xdr:colOff>10800</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>153360</xdr:rowOff>
     </xdr:from>
@@ -2230,8 +2357,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13917240" y="478440"/>
-          <a:ext cx="559800" cy="0"/>
+          <a:off x="14050440" y="478440"/>
+          <a:ext cx="559440" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2255,7 +2382,7 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>44</xdr:col>
-      <xdr:colOff>2160</xdr:colOff>
+      <xdr:colOff>2520</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>153000</xdr:rowOff>
     </xdr:from>
@@ -2272,7 +2399,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15261840" y="478080"/>
+          <a:off x="15394680" y="478080"/>
           <a:ext cx="556560" cy="3600"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2297,15 +2424,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>49</xdr:col>
-      <xdr:colOff>20520</xdr:colOff>
+      <xdr:colOff>21240</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>160200</xdr:rowOff>
+      <xdr:rowOff>160560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>51</xdr:col>
-      <xdr:colOff>9000</xdr:colOff>
+      <xdr:colOff>9720</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>3240</xdr:rowOff>
+      <xdr:rowOff>3600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2314,8 +2441,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="16632720" y="484920"/>
-          <a:ext cx="529200" cy="5400"/>
+          <a:off x="16765560" y="485280"/>
+          <a:ext cx="529560" cy="5400"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2339,15 +2466,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>53</xdr:col>
-      <xdr:colOff>250920</xdr:colOff>
+      <xdr:colOff>251280</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>155520</xdr:rowOff>
+      <xdr:rowOff>155880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>56</xdr:col>
-      <xdr:colOff>19800</xdr:colOff>
+      <xdr:colOff>20520</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>156600</xdr:rowOff>
+      <xdr:rowOff>156960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2356,7 +2483,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17944560" y="480240"/>
+          <a:off x="18077760" y="480600"/>
           <a:ext cx="580680" cy="1080"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2381,15 +2508,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>58</xdr:col>
-      <xdr:colOff>251640</xdr:colOff>
+      <xdr:colOff>252000</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>156600</xdr:rowOff>
+      <xdr:rowOff>156960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>60</xdr:col>
-      <xdr:colOff>262080</xdr:colOff>
+      <xdr:colOff>262440</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>3240</xdr:rowOff>
+      <xdr:rowOff>3600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2398,7 +2525,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="19298160" y="481320"/>
+          <a:off x="19431360" y="481680"/>
           <a:ext cx="551520" cy="9000"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2423,15 +2550,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>64</xdr:col>
-      <xdr:colOff>1440</xdr:colOff>
+      <xdr:colOff>1800</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>156600</xdr:rowOff>
+      <xdr:rowOff>156960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>66</xdr:col>
-      <xdr:colOff>1440</xdr:colOff>
+      <xdr:colOff>2160</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>3240</xdr:rowOff>
+      <xdr:rowOff>3600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2440,7 +2567,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="20670840" y="481320"/>
+          <a:off x="20804040" y="481680"/>
           <a:ext cx="541080" cy="9000"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2465,15 +2592,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>64</xdr:col>
-      <xdr:colOff>263160</xdr:colOff>
+      <xdr:colOff>263520</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>2880</xdr:rowOff>
+      <xdr:rowOff>3240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>64</xdr:col>
-      <xdr:colOff>269280</xdr:colOff>
+      <xdr:colOff>269640</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>2520</xdr:rowOff>
+      <xdr:rowOff>2880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2482,7 +2609,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="20932560" y="490320"/>
+          <a:off x="21065760" y="490680"/>
           <a:ext cx="6120" cy="1950480"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2509,13 +2636,13 @@
       <xdr:col>19</xdr:col>
       <xdr:colOff>7920</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>160200</xdr:rowOff>
+      <xdr:rowOff>160560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>259920</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>3960</xdr:rowOff>
+      <xdr:rowOff>4320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2524,7 +2651,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="8504640" y="484920"/>
+          <a:off x="8637480" y="485280"/>
           <a:ext cx="252000" cy="6120"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2549,15 +2676,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>28</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>268920</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>-360</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>64</xdr:col>
-      <xdr:colOff>254160</xdr:colOff>
+      <xdr:colOff>254520</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>5760</xdr:rowOff>
+      <xdr:rowOff>6120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2566,7 +2693,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11199600" y="2437560"/>
+          <a:off x="11332800" y="2437920"/>
           <a:ext cx="9723960" cy="6120"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2598,11 +2725,11 @@
   </sheetPr>
   <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.94921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.96484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.77"/>
   </cols>
@@ -3143,18 +3270,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BQ18"/>
+  <dimension ref="A1:BQ35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="10" ySplit="0" topLeftCell="K10" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="topRight" activeCell="A32" activeCellId="0" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
   <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="20" width="11.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="16.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="8" min="7" style="3" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="9" min="9" style="20" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="9" min="9" style="21" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="3" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="107" min="11" style="0" width="3.83"/>
   </cols>
@@ -3163,27 +3294,27 @@
       <c r="A1" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="21" t="s">
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="I1" s="22" t="s">
+      <c r="I1" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="23" t="s">
         <v>51</v>
       </c>
     </row>
@@ -3191,330 +3322,510 @@
       <c r="A2" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="24" t="s">
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="G2" s="25" t="n">
+      <c r="G2" s="28" t="n">
         <v>5</v>
       </c>
-      <c r="H2" s="24" t="s">
+      <c r="H2" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="I2" s="26" t="n">
+      <c r="I2" s="29" t="n">
         <v>1</v>
       </c>
-      <c r="J2" s="25" t="n">
+      <c r="J2" s="28" t="n">
         <f aca="false">ROUND(G2/(H2*I2),0)</f>
         <v>5</v>
       </c>
-      <c r="L2" s="27" t="n">
+      <c r="L2" s="30" t="n">
         <v>0</v>
       </c>
-      <c r="M2" s="28"/>
-      <c r="N2" s="27"/>
-      <c r="Q2" s="27"/>
-      <c r="R2" s="28"/>
-      <c r="S2" s="27"/>
-      <c r="V2" s="27"/>
-      <c r="W2" s="28"/>
-      <c r="X2" s="27"/>
-      <c r="AF2" s="27"/>
-      <c r="AG2" s="28"/>
-      <c r="AH2" s="27"/>
-      <c r="AK2" s="27"/>
-      <c r="AL2" s="28"/>
-      <c r="AM2" s="27"/>
-      <c r="AP2" s="27"/>
-      <c r="AQ2" s="28"/>
-      <c r="AR2" s="27"/>
-      <c r="AU2" s="27"/>
-      <c r="AV2" s="28"/>
-      <c r="AW2" s="27"/>
-      <c r="AZ2" s="27"/>
-      <c r="BA2" s="28"/>
-      <c r="BB2" s="27"/>
-      <c r="BE2" s="27"/>
-      <c r="BF2" s="28"/>
-      <c r="BG2" s="27"/>
-      <c r="BJ2" s="27"/>
-      <c r="BK2" s="28"/>
-      <c r="BL2" s="27"/>
-      <c r="BO2" s="27"/>
-      <c r="BP2" s="28"/>
-      <c r="BQ2" s="27"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="30" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q2" s="30" t="n">
+        <v>5</v>
+      </c>
+      <c r="R2" s="31"/>
+      <c r="S2" s="30" t="n">
+        <v>6</v>
+      </c>
+      <c r="V2" s="30" t="n">
+        <v>6</v>
+      </c>
+      <c r="W2" s="31"/>
+      <c r="X2" s="30" t="n">
+        <v>10</v>
+      </c>
+      <c r="AF2" s="30" t="n">
+        <v>16</v>
+      </c>
+      <c r="AG2" s="31"/>
+      <c r="AH2" s="30" t="n">
+        <v>18</v>
+      </c>
+      <c r="AK2" s="30" t="n">
+        <f aca="false">AH2</f>
+        <v>18</v>
+      </c>
+      <c r="AL2" s="31"/>
+      <c r="AM2" s="30" t="n">
+        <f aca="false">AK2+AK4</f>
+        <v>20</v>
+      </c>
+      <c r="AP2" s="30" t="n">
+        <f aca="false">AM2</f>
+        <v>20</v>
+      </c>
+      <c r="AQ2" s="31"/>
+      <c r="AR2" s="30" t="n">
+        <f aca="false">AP2+AP4</f>
+        <v>22</v>
+      </c>
+      <c r="AU2" s="30" t="n">
+        <f aca="false">AR2</f>
+        <v>22</v>
+      </c>
+      <c r="AV2" s="31"/>
+      <c r="AW2" s="30" t="n">
+        <f aca="false">AU2+AU4</f>
+        <v>25</v>
+      </c>
+      <c r="AZ2" s="30" t="n">
+        <f aca="false">AW2</f>
+        <v>25</v>
+      </c>
+      <c r="BA2" s="31"/>
+      <c r="BB2" s="30" t="n">
+        <f aca="false">AZ2+AZ4</f>
+        <v>27</v>
+      </c>
+      <c r="BE2" s="30" t="n">
+        <f aca="false">BB2</f>
+        <v>27</v>
+      </c>
+      <c r="BF2" s="31"/>
+      <c r="BG2" s="30" t="n">
+        <f aca="false">BE2+BE4</f>
+        <v>28</v>
+      </c>
+      <c r="BJ2" s="30" t="n">
+        <f aca="false">BG2</f>
+        <v>28</v>
+      </c>
+      <c r="BK2" s="31"/>
+      <c r="BL2" s="30" t="n">
+        <f aca="false">BJ2+BJ4</f>
+        <v>33</v>
+      </c>
+      <c r="BO2" s="30" t="n">
+        <f aca="false">MAX(BL2,AC14)</f>
+        <v>33</v>
+      </c>
+      <c r="BP2" s="31"/>
+      <c r="BQ2" s="30" t="n">
+        <f aca="false">BO2+BO4</f>
+        <v>34</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="29" t="s">
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="29" t="s">
+      <c r="F3" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="G3" s="30" t="n">
+      <c r="G3" s="34" t="n">
         <v>1</v>
       </c>
-      <c r="H3" s="29" t="s">
+      <c r="H3" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="I3" s="31" t="n">
+      <c r="I3" s="35" t="n">
         <v>1</v>
       </c>
-      <c r="J3" s="30" t="n">
+      <c r="J3" s="34" t="n">
         <f aca="false">ROUND(G3/(H3*I3),0)</f>
         <v>1</v>
       </c>
-      <c r="L3" s="32" t="s">
+      <c r="L3" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="M3" s="32"/>
-      <c r="N3" s="32"/>
-      <c r="Q3" s="32" t="s">
+      <c r="M3" s="36"/>
+      <c r="N3" s="36"/>
+      <c r="Q3" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="R3" s="32"/>
-      <c r="S3" s="32"/>
-      <c r="V3" s="32" t="s">
+      <c r="R3" s="36"/>
+      <c r="S3" s="36"/>
+      <c r="V3" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="W3" s="32"/>
-      <c r="X3" s="32"/>
-      <c r="AF3" s="32" t="s">
+      <c r="W3" s="36"/>
+      <c r="X3" s="36"/>
+      <c r="AF3" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="AG3" s="32"/>
-      <c r="AH3" s="32"/>
-      <c r="AK3" s="32" t="s">
+      <c r="AG3" s="36"/>
+      <c r="AH3" s="36"/>
+      <c r="AK3" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="AL3" s="32"/>
-      <c r="AM3" s="32"/>
-      <c r="AP3" s="32" t="s">
+      <c r="AL3" s="36"/>
+      <c r="AM3" s="36"/>
+      <c r="AP3" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="AQ3" s="32"/>
-      <c r="AR3" s="32"/>
-      <c r="AU3" s="32" t="s">
+      <c r="AQ3" s="36"/>
+      <c r="AR3" s="36"/>
+      <c r="AU3" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="AV3" s="32"/>
-      <c r="AW3" s="32"/>
-      <c r="AZ3" s="32" t="s">
+      <c r="AV3" s="36"/>
+      <c r="AW3" s="36"/>
+      <c r="AZ3" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="BA3" s="32"/>
-      <c r="BB3" s="32"/>
-      <c r="BE3" s="32" t="s">
+      <c r="BA3" s="36"/>
+      <c r="BB3" s="36"/>
+      <c r="BE3" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="BF3" s="32"/>
-      <c r="BG3" s="32"/>
-      <c r="BJ3" s="32" t="s">
+      <c r="BF3" s="36"/>
+      <c r="BG3" s="36"/>
+      <c r="BJ3" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="BK3" s="32"/>
-      <c r="BL3" s="32"/>
-      <c r="BO3" s="32" t="s">
+      <c r="BK3" s="36"/>
+      <c r="BL3" s="36"/>
+      <c r="BO3" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="BP3" s="32"/>
-      <c r="BQ3" s="32"/>
+      <c r="BP3" s="36"/>
+      <c r="BQ3" s="36"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="29" t="s">
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="29" t="s">
+      <c r="F4" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="G4" s="30" t="n">
+      <c r="G4" s="34" t="n">
         <v>4</v>
       </c>
-      <c r="H4" s="29" t="s">
+      <c r="H4" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="I4" s="31" t="n">
+      <c r="I4" s="35" t="n">
         <v>1</v>
       </c>
-      <c r="J4" s="30" t="n">
+      <c r="J4" s="34" t="n">
         <f aca="false">ROUND(G4/(H4*I4),0)</f>
         <v>4</v>
       </c>
-      <c r="L4" s="33" t="n">
+      <c r="L4" s="37" t="n">
         <f aca="false">VLOOKUP(L3,$A$2:$J$17,10)</f>
         <v>5</v>
       </c>
-      <c r="M4" s="34"/>
-      <c r="N4" s="33"/>
-      <c r="Q4" s="33" t="n">
+      <c r="M4" s="38" t="n">
+        <f aca="false">N5-N2</f>
+        <v>0</v>
+      </c>
+      <c r="N4" s="37" t="n">
+        <f aca="false">MIN(Q2,Q14)-N2</f>
+        <v>0</v>
+      </c>
+      <c r="Q4" s="37" t="n">
         <f aca="false">VLOOKUP(Q3,$A$2:$J$17,10)</f>
         <v>1</v>
       </c>
-      <c r="R4" s="34"/>
-      <c r="S4" s="33"/>
-      <c r="V4" s="33" t="n">
+      <c r="R4" s="38" t="n">
+        <f aca="false">S5-S2</f>
+        <v>0</v>
+      </c>
+      <c r="S4" s="37" t="n">
+        <f aca="false">MIN(V2,V8)-S2</f>
+        <v>0</v>
+      </c>
+      <c r="V4" s="37" t="n">
         <f aca="false">VLOOKUP(V3,$A$2:$J$17,10)</f>
         <v>4</v>
       </c>
-      <c r="W4" s="34"/>
-      <c r="X4" s="33"/>
-      <c r="AF4" s="33" t="n">
+      <c r="W4" s="38" t="n">
+        <f aca="false">X5-X2</f>
+        <v>6</v>
+      </c>
+      <c r="X4" s="38" t="n">
+        <f aca="false">AF2-X2</f>
+        <v>6</v>
+      </c>
+      <c r="AF4" s="37" t="n">
         <f aca="false">VLOOKUP(AF3,$A$2:$J$17,10)</f>
         <v>2</v>
       </c>
-      <c r="AG4" s="34"/>
-      <c r="AH4" s="33"/>
-      <c r="AK4" s="33" t="n">
+      <c r="AG4" s="38" t="n">
+        <f aca="false">AH5-AH2</f>
+        <v>0</v>
+      </c>
+      <c r="AH4" s="37" t="n">
+        <f aca="false">AK2-AH2</f>
+        <v>0</v>
+      </c>
+      <c r="AK4" s="37" t="n">
         <f aca="false">VLOOKUP(AK3,$A$2:$J$17,10)</f>
         <v>2</v>
       </c>
-      <c r="AL4" s="34"/>
-      <c r="AM4" s="33"/>
-      <c r="AP4" s="33" t="n">
+      <c r="AL4" s="38" t="n">
+        <f aca="false">AM5-AM2</f>
+        <v>0</v>
+      </c>
+      <c r="AM4" s="37" t="n">
+        <f aca="false">AP2-AM2</f>
+        <v>0</v>
+      </c>
+      <c r="AP4" s="37" t="n">
         <f aca="false">VLOOKUP(AP3,$A$2:$J$17,10)</f>
         <v>2</v>
       </c>
-      <c r="AQ4" s="34"/>
-      <c r="AR4" s="33"/>
-      <c r="AU4" s="33" t="n">
+      <c r="AQ4" s="38" t="n">
+        <f aca="false">AR5-AR2</f>
+        <v>0</v>
+      </c>
+      <c r="AR4" s="37" t="n">
+        <f aca="false">AU2-AR2</f>
+        <v>0</v>
+      </c>
+      <c r="AU4" s="37" t="n">
         <f aca="false">VLOOKUP(AU3,$A$2:$J$17,10)</f>
         <v>3</v>
       </c>
-      <c r="AV4" s="34"/>
-      <c r="AW4" s="33"/>
-      <c r="AZ4" s="33" t="n">
+      <c r="AV4" s="38" t="n">
+        <f aca="false">AW5-AW2</f>
+        <v>0</v>
+      </c>
+      <c r="AW4" s="37" t="n">
+        <f aca="false">AZ2-AW2</f>
+        <v>0</v>
+      </c>
+      <c r="AZ4" s="37" t="n">
         <f aca="false">VLOOKUP(AZ3,$A$2:$J$17,10)</f>
         <v>2</v>
       </c>
-      <c r="BA4" s="34"/>
-      <c r="BB4" s="33"/>
-      <c r="BE4" s="33" t="n">
+      <c r="BA4" s="38" t="n">
+        <f aca="false">BB5-BB2</f>
+        <v>0</v>
+      </c>
+      <c r="BB4" s="37" t="n">
+        <f aca="false">BE2-BB2</f>
+        <v>0</v>
+      </c>
+      <c r="BE4" s="37" t="n">
         <f aca="false">VLOOKUP(BE3,$A$2:$J$17,10)</f>
         <v>1</v>
       </c>
-      <c r="BF4" s="34"/>
-      <c r="BG4" s="33"/>
-      <c r="BJ4" s="33" t="n">
+      <c r="BF4" s="38" t="n">
+        <f aca="false">BG5-BG2</f>
+        <v>0</v>
+      </c>
+      <c r="BG4" s="37" t="n">
+        <f aca="false">BJ2-BG2</f>
+        <v>0</v>
+      </c>
+      <c r="BJ4" s="37" t="n">
         <v>5</v>
       </c>
-      <c r="BK4" s="34"/>
-      <c r="BL4" s="33"/>
-      <c r="BO4" s="33" t="n">
+      <c r="BK4" s="38" t="n">
+        <f aca="false">BL5-BL2</f>
+        <v>0</v>
+      </c>
+      <c r="BL4" s="37" t="n">
+        <f aca="false">BO2-BL2</f>
+        <v>0</v>
+      </c>
+      <c r="BO4" s="37" t="n">
         <v>1</v>
       </c>
-      <c r="BP4" s="34"/>
-      <c r="BQ4" s="33"/>
+      <c r="BP4" s="38" t="n">
+        <f aca="false">BQ5-BQ2</f>
+        <v>0</v>
+      </c>
+      <c r="BQ4" s="37"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="29" t="s">
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="29" t="s">
+      <c r="F5" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="30" t="n">
+      <c r="G5" s="34" t="n">
         <v>3</v>
       </c>
-      <c r="H5" s="29" t="s">
+      <c r="H5" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="I5" s="31" t="n">
+      <c r="I5" s="35" t="n">
         <v>1</v>
       </c>
-      <c r="J5" s="30" t="n">
+      <c r="J5" s="34" t="n">
         <f aca="false">ROUND(G5/(H5*I5),0)</f>
         <v>3</v>
       </c>
-      <c r="L5" s="27" t="n">
+      <c r="L5" s="30" t="n">
         <v>0</v>
       </c>
-      <c r="M5" s="28"/>
-      <c r="N5" s="27"/>
-      <c r="Q5" s="27"/>
-      <c r="R5" s="28"/>
-      <c r="S5" s="27"/>
-      <c r="V5" s="27"/>
-      <c r="W5" s="28"/>
-      <c r="X5" s="27"/>
-      <c r="AF5" s="27"/>
-      <c r="AG5" s="28"/>
-      <c r="AH5" s="27"/>
-      <c r="AK5" s="27"/>
-      <c r="AL5" s="28"/>
-      <c r="AM5" s="27"/>
-      <c r="AP5" s="27"/>
-      <c r="AQ5" s="28"/>
-      <c r="AR5" s="27"/>
-      <c r="AU5" s="27"/>
-      <c r="AV5" s="28"/>
-      <c r="AW5" s="27"/>
-      <c r="AZ5" s="27"/>
-      <c r="BA5" s="28"/>
-      <c r="BB5" s="27"/>
-      <c r="BE5" s="27"/>
-      <c r="BF5" s="28"/>
-      <c r="BG5" s="27"/>
-      <c r="BJ5" s="27"/>
-      <c r="BK5" s="28"/>
-      <c r="BL5" s="27"/>
-      <c r="BO5" s="27"/>
-      <c r="BP5" s="28"/>
-      <c r="BQ5" s="27"/>
+      <c r="M5" s="31"/>
+      <c r="N5" s="30" t="n">
+        <f aca="false">MIN(Q5,Q17)</f>
+        <v>5</v>
+      </c>
+      <c r="Q5" s="30" t="n">
+        <f aca="false">S5-Q4</f>
+        <v>5</v>
+      </c>
+      <c r="R5" s="31"/>
+      <c r="S5" s="30" t="n">
+        <f aca="false">MIN(V5,V11)</f>
+        <v>6</v>
+      </c>
+      <c r="V5" s="30" t="n">
+        <f aca="false">X5-V4</f>
+        <v>12</v>
+      </c>
+      <c r="W5" s="31"/>
+      <c r="X5" s="30" t="n">
+        <v>16</v>
+      </c>
+      <c r="AF5" s="30" t="n">
+        <f aca="false">AH5-AF4</f>
+        <v>16</v>
+      </c>
+      <c r="AG5" s="31"/>
+      <c r="AH5" s="30" t="n">
+        <f aca="false">AK5</f>
+        <v>18</v>
+      </c>
+      <c r="AK5" s="30" t="n">
+        <f aca="false">AM5-AK4</f>
+        <v>18</v>
+      </c>
+      <c r="AL5" s="31"/>
+      <c r="AM5" s="30" t="n">
+        <f aca="false">AP5</f>
+        <v>20</v>
+      </c>
+      <c r="AP5" s="30" t="n">
+        <f aca="false">AR5-AP4</f>
+        <v>20</v>
+      </c>
+      <c r="AQ5" s="31"/>
+      <c r="AR5" s="30" t="n">
+        <f aca="false">AU5</f>
+        <v>22</v>
+      </c>
+      <c r="AU5" s="30" t="n">
+        <f aca="false">AW5-AU4</f>
+        <v>22</v>
+      </c>
+      <c r="AV5" s="31"/>
+      <c r="AW5" s="30" t="n">
+        <f aca="false">AZ5</f>
+        <v>25</v>
+      </c>
+      <c r="AZ5" s="30" t="n">
+        <f aca="false">BB5-AZ4</f>
+        <v>25</v>
+      </c>
+      <c r="BA5" s="31"/>
+      <c r="BB5" s="30" t="n">
+        <f aca="false">BE5</f>
+        <v>27</v>
+      </c>
+      <c r="BE5" s="30" t="n">
+        <f aca="false">BG5-BE4</f>
+        <v>27</v>
+      </c>
+      <c r="BF5" s="31"/>
+      <c r="BG5" s="30" t="n">
+        <f aca="false">BJ5</f>
+        <v>28</v>
+      </c>
+      <c r="BJ5" s="30" t="n">
+        <f aca="false">BL5-BJ4</f>
+        <v>28</v>
+      </c>
+      <c r="BK5" s="31"/>
+      <c r="BL5" s="30" t="n">
+        <v>33</v>
+      </c>
+      <c r="BO5" s="30" t="n">
+        <f aca="false">BQ5-BO4</f>
+        <v>33</v>
+      </c>
+      <c r="BP5" s="31"/>
+      <c r="BQ5" s="30" t="n">
+        <f aca="false">BQ2</f>
+        <v>34</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="35" t="s">
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="35" t="s">
+      <c r="F6" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="G6" s="36" t="n">
+      <c r="G6" s="40" t="n">
         <v>7</v>
       </c>
-      <c r="H6" s="29" t="s">
+      <c r="H6" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="I6" s="31" t="n">
+      <c r="I6" s="35" t="n">
         <v>1</v>
       </c>
-      <c r="J6" s="30" t="n">
+      <c r="J6" s="34" t="n">
         <f aca="false">ROUND(G6/(H6*I6),0)</f>
         <v>7</v>
       </c>
@@ -3523,27 +3834,27 @@
       <c r="A7" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="29" t="s">
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="29" t="s">
+      <c r="F7" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="30" t="n">
+      <c r="G7" s="34" t="n">
         <v>1</v>
       </c>
-      <c r="H7" s="29" t="s">
+      <c r="H7" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="I7" s="31" t="n">
+      <c r="I7" s="35" t="n">
         <v>1</v>
       </c>
-      <c r="J7" s="30" t="n">
+      <c r="J7" s="34" t="n">
         <f aca="false">ROUND(G7/(H7*I7),0)</f>
         <v>1</v>
       </c>
@@ -3552,189 +3863,207 @@
       <c r="A8" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="35" t="s">
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="35" t="s">
+      <c r="F8" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="G8" s="36" t="n">
+      <c r="G8" s="40" t="n">
         <v>3</v>
       </c>
-      <c r="H8" s="29" t="s">
+      <c r="H8" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="I8" s="31" t="n">
+      <c r="I8" s="35" t="n">
         <v>1</v>
       </c>
-      <c r="J8" s="30" t="n">
+      <c r="J8" s="34" t="n">
         <f aca="false">ROUND(G8/(H8*I8),0)</f>
         <v>3</v>
       </c>
-      <c r="V8" s="27" t="n">
-        <f aca="false">S2</f>
-        <v>0</v>
-      </c>
-      <c r="W8" s="28"/>
-      <c r="X8" s="27" t="n">
-        <f aca="false">V8+V10</f>
-        <v>3</v>
-      </c>
-      <c r="AA8" s="27" t="n">
-        <f aca="false">X8</f>
-        <v>3</v>
-      </c>
-      <c r="AB8" s="28"/>
-      <c r="AC8" s="27" t="n">
-        <f aca="false">AA8+AA10</f>
-        <v>10</v>
+      <c r="V8" s="30" t="n">
+        <v>6</v>
+      </c>
+      <c r="W8" s="31"/>
+      <c r="X8" s="30" t="n">
+        <v>9</v>
+      </c>
+      <c r="AA8" s="30" t="n">
+        <v>9</v>
+      </c>
+      <c r="AB8" s="31"/>
+      <c r="AC8" s="30" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="35" t="s">
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="F9" s="35" t="s">
+      <c r="F9" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="G9" s="36" t="n">
+      <c r="G9" s="40" t="n">
         <v>2</v>
       </c>
-      <c r="H9" s="29" t="s">
+      <c r="H9" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="I9" s="31" t="n">
+      <c r="I9" s="35" t="n">
         <v>1</v>
       </c>
-      <c r="J9" s="30" t="n">
+      <c r="J9" s="34" t="n">
         <f aca="false">ROUND(G9/(H9*I9),0)</f>
         <v>2</v>
       </c>
-      <c r="V9" s="32" t="s">
+      <c r="V9" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="W9" s="32"/>
-      <c r="X9" s="32"/>
-      <c r="AA9" s="32" t="s">
+      <c r="W9" s="36"/>
+      <c r="X9" s="36"/>
+      <c r="AA9" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="AB9" s="32"/>
-      <c r="AC9" s="32"/>
+      <c r="AB9" s="36"/>
+      <c r="AC9" s="36"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="35" t="s">
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="35" t="s">
+      <c r="F10" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="G10" s="36" t="n">
+      <c r="G10" s="40" t="n">
         <v>2</v>
       </c>
-      <c r="H10" s="29" t="s">
+      <c r="H10" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="I10" s="31" t="n">
+      <c r="I10" s="35" t="n">
         <v>1</v>
       </c>
-      <c r="J10" s="30" t="n">
+      <c r="J10" s="34" t="n">
         <f aca="false">ROUND(G10/(H10*I10),0)</f>
         <v>2</v>
       </c>
-      <c r="V10" s="33" t="n">
+      <c r="V10" s="37" t="n">
         <f aca="false">VLOOKUP(V9,$A$2:$J$17,10)</f>
         <v>3</v>
       </c>
-      <c r="W10" s="34"/>
-      <c r="X10" s="33"/>
-      <c r="AA10" s="33" t="n">
+      <c r="W10" s="38" t="n">
+        <f aca="false">X11-X8</f>
+        <v>0</v>
+      </c>
+      <c r="X10" s="37" t="n">
+        <f aca="false">AA8-X8</f>
+        <v>0</v>
+      </c>
+      <c r="AA10" s="37" t="n">
         <f aca="false">VLOOKUP(AA9,$A$2:$J$17,10)</f>
         <v>7</v>
       </c>
-      <c r="AB10" s="34"/>
-      <c r="AC10" s="33"/>
+      <c r="AB10" s="38" t="n">
+        <f aca="false">AC11-AC8</f>
+        <v>0</v>
+      </c>
+      <c r="AC10" s="37" t="n">
+        <f aca="false">AF2-AC8</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="35" t="s">
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="F11" s="35" t="s">
+      <c r="F11" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="36" t="n">
+      <c r="G11" s="40" t="n">
         <v>2</v>
       </c>
-      <c r="H11" s="29" t="s">
+      <c r="H11" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="I11" s="31" t="n">
+      <c r="I11" s="35" t="n">
         <v>1</v>
       </c>
-      <c r="J11" s="30" t="n">
+      <c r="J11" s="34" t="n">
         <f aca="false">ROUND(G11/(H11*I11),0)</f>
         <v>2</v>
       </c>
-      <c r="V11" s="27"/>
-      <c r="W11" s="28"/>
-      <c r="X11" s="27"/>
-      <c r="AA11" s="27"/>
-      <c r="AB11" s="28"/>
-      <c r="AC11" s="27"/>
+      <c r="V11" s="30" t="n">
+        <f aca="false">X11-V10</f>
+        <v>6</v>
+      </c>
+      <c r="W11" s="31"/>
+      <c r="X11" s="30" t="n">
+        <v>9</v>
+      </c>
+      <c r="AA11" s="30" t="n">
+        <f aca="false">AC11-AA10</f>
+        <v>9</v>
+      </c>
+      <c r="AB11" s="31"/>
+      <c r="AC11" s="30" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="35" t="s">
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="F12" s="35" t="s">
+      <c r="F12" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="G12" s="36" t="n">
+      <c r="G12" s="40" t="n">
         <v>10</v>
       </c>
-      <c r="H12" s="29" t="s">
+      <c r="H12" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="I12" s="31" t="n">
+      <c r="I12" s="35" t="n">
         <v>1</v>
       </c>
-      <c r="J12" s="30" t="n">
+      <c r="J12" s="34" t="n">
         <f aca="false">ROUND(G12/(H12*I12),0)</f>
         <v>10</v>
       </c>
@@ -3743,27 +4072,27 @@
       <c r="A13" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="35" t="s">
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="F13" s="35" t="s">
+      <c r="F13" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="G13" s="36" t="n">
+      <c r="G13" s="40" t="n">
         <v>3</v>
       </c>
-      <c r="H13" s="29" t="s">
+      <c r="H13" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="I13" s="31" t="n">
+      <c r="I13" s="35" t="n">
         <v>1</v>
       </c>
-      <c r="J13" s="30" t="n">
+      <c r="J13" s="34" t="n">
         <f aca="false">ROUND(G13/(H13*I13),0)</f>
         <v>3</v>
       </c>
@@ -3772,174 +4101,356 @@
       <c r="A14" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="35" t="s">
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="35" t="s">
+      <c r="F14" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="G14" s="36" t="n">
+      <c r="G14" s="40" t="n">
         <v>3</v>
       </c>
-      <c r="H14" s="29" t="s">
+      <c r="H14" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="I14" s="31" t="n">
+      <c r="I14" s="35" t="n">
         <v>1</v>
       </c>
-      <c r="J14" s="30" t="n">
+      <c r="J14" s="34" t="n">
         <f aca="false">ROUND(G14/(H14*I14),0)</f>
         <v>3</v>
       </c>
-      <c r="Q14" s="27"/>
-      <c r="R14" s="28"/>
-      <c r="S14" s="27"/>
-      <c r="V14" s="27"/>
-      <c r="W14" s="28"/>
-      <c r="X14" s="27"/>
-      <c r="AA14" s="27"/>
-      <c r="AB14" s="28"/>
-      <c r="AC14" s="27"/>
+      <c r="Q14" s="30" t="n">
+        <v>5</v>
+      </c>
+      <c r="R14" s="31"/>
+      <c r="S14" s="30" t="n">
+        <v>6</v>
+      </c>
+      <c r="V14" s="30" t="n">
+        <v>6</v>
+      </c>
+      <c r="W14" s="31"/>
+      <c r="X14" s="30" t="n">
+        <v>9</v>
+      </c>
+      <c r="AA14" s="30" t="n">
+        <v>9</v>
+      </c>
+      <c r="AB14" s="31"/>
+      <c r="AC14" s="30" t="n">
+        <v>19</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="35" t="s">
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="F15" s="35" t="s">
+      <c r="F15" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="G15" s="36" t="n">
+      <c r="G15" s="40" t="n">
         <v>1</v>
       </c>
-      <c r="H15" s="29" t="s">
+      <c r="H15" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="I15" s="31" t="n">
+      <c r="I15" s="35" t="n">
         <v>1</v>
       </c>
-      <c r="J15" s="30" t="n">
+      <c r="J15" s="34" t="n">
         <f aca="false">ROUND(G15/(H15*I15),0)</f>
         <v>1</v>
       </c>
-      <c r="Q15" s="32" t="s">
+      <c r="Q15" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="R15" s="32"/>
-      <c r="S15" s="32"/>
-      <c r="V15" s="32" t="s">
+      <c r="R15" s="36"/>
+      <c r="S15" s="36"/>
+      <c r="V15" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="W15" s="32"/>
-      <c r="X15" s="32"/>
-      <c r="AA15" s="32" t="s">
+      <c r="W15" s="36"/>
+      <c r="X15" s="36"/>
+      <c r="AA15" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="AB15" s="32"/>
-      <c r="AC15" s="32"/>
+      <c r="AB15" s="36"/>
+      <c r="AC15" s="36"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="35" t="s">
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="F16" s="35" t="s">
+      <c r="F16" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="G16" s="36" t="n">
+      <c r="G16" s="40" t="n">
         <v>5</v>
       </c>
-      <c r="H16" s="29" t="s">
+      <c r="H16" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="I16" s="31" t="n">
+      <c r="I16" s="35" t="n">
         <v>1</v>
       </c>
-      <c r="J16" s="30" t="n">
+      <c r="J16" s="34" t="n">
         <f aca="false">ROUND(G16/(H16*I16),0)</f>
         <v>5</v>
       </c>
-      <c r="Q16" s="33" t="n">
+      <c r="Q16" s="37" t="n">
         <f aca="false">VLOOKUP(Q15,$A$2:$J$17,10)</f>
         <v>1</v>
       </c>
-      <c r="R16" s="34"/>
-      <c r="S16" s="33"/>
-      <c r="V16" s="33" t="n">
+      <c r="R16" s="38" t="n">
+        <f aca="false">S17-S14</f>
+        <v>7</v>
+      </c>
+      <c r="S16" s="37" t="n">
+        <f aca="false">V14-S14</f>
+        <v>0</v>
+      </c>
+      <c r="V16" s="37" t="n">
         <f aca="false">VLOOKUP(V15,$A$2:$J$17,10)</f>
         <v>3</v>
       </c>
-      <c r="W16" s="34"/>
-      <c r="X16" s="33"/>
-      <c r="AA16" s="33" t="n">
+      <c r="W16" s="38" t="n">
+        <f aca="false">X17-X14</f>
+        <v>7</v>
+      </c>
+      <c r="X16" s="37" t="n">
+        <f aca="false">MIN(AA14,AF2)-X14</f>
+        <v>0</v>
+      </c>
+      <c r="AA16" s="37" t="n">
         <f aca="false">VLOOKUP(AA15,$A$2:$J$17,10)</f>
         <v>10</v>
       </c>
-      <c r="AB16" s="34"/>
-      <c r="AC16" s="33"/>
+      <c r="AB16" s="38" t="n">
+        <f aca="false">AC17-AC14</f>
+        <v>14</v>
+      </c>
+      <c r="AC16" s="38" t="n">
+        <f aca="false">BO2-AC14</f>
+        <v>14</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="37" t="s">
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="F17" s="38"/>
-      <c r="G17" s="39" t="n">
+      <c r="F17" s="43"/>
+      <c r="G17" s="44" t="n">
         <v>1</v>
       </c>
-      <c r="H17" s="37" t="s">
+      <c r="H17" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="I17" s="31" t="n">
+      <c r="I17" s="35" t="n">
         <v>1</v>
       </c>
-      <c r="J17" s="39" t="n">
+      <c r="J17" s="44" t="n">
         <f aca="false">ROUND(G17/(H17*I17),0)</f>
         <v>1</v>
       </c>
-      <c r="Q17" s="27"/>
-      <c r="R17" s="28"/>
-      <c r="S17" s="27"/>
-      <c r="V17" s="27"/>
-      <c r="W17" s="28"/>
-      <c r="X17" s="27"/>
-      <c r="AA17" s="27"/>
-      <c r="AB17" s="28"/>
-      <c r="AC17" s="27"/>
+      <c r="Q17" s="30" t="n">
+        <f aca="false">S17-Q16</f>
+        <v>12</v>
+      </c>
+      <c r="R17" s="31"/>
+      <c r="S17" s="30" t="n">
+        <f aca="false">V17</f>
+        <v>13</v>
+      </c>
+      <c r="V17" s="30" t="n">
+        <f aca="false">X17-V16</f>
+        <v>13</v>
+      </c>
+      <c r="W17" s="31"/>
+      <c r="X17" s="30" t="n">
+        <f aca="false">MIN(AF5,AA17)</f>
+        <v>16</v>
+      </c>
+      <c r="AA17" s="30" t="n">
+        <f aca="false">AC17-AA16</f>
+        <v>23</v>
+      </c>
+      <c r="AB17" s="31"/>
+      <c r="AC17" s="30" t="n">
+        <v>33</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G18" s="28"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="28"/>
+      <c r="G18" s="31"/>
+      <c r="H18" s="31"/>
+      <c r="I18" s="31"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="45" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" s="46" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="47"/>
+      <c r="D19" s="48" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="36"/>
+      <c r="D20" s="36"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="D21" s="37" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="49" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" s="50" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" s="51"/>
+      <c r="D22" s="52" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="53" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" s="31"/>
+      <c r="D24" s="30" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="C25" s="36"/>
+      <c r="D25" s="36"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="C26" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="D26" s="37" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="C27" s="31"/>
+      <c r="D27" s="30" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29" s="54" t="s">
+        <v>73</v>
+      </c>
+      <c r="C29" s="55" t="s">
+        <v>74</v>
+      </c>
+      <c r="D29" s="55"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" s="54" t="s">
+        <v>73</v>
+      </c>
+      <c r="C30" s="55" t="s">
+        <v>75</v>
+      </c>
+      <c r="D30" s="55"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="54"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="B32" s="54" t="s">
+        <v>73</v>
+      </c>
+      <c r="C32" s="55" t="s">
+        <v>75</v>
+      </c>
+      <c r="D32" s="55"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="B33" s="54" t="s">
+        <v>73</v>
+      </c>
+      <c r="C33" s="55" t="s">
+        <v>74</v>
+      </c>
+      <c r="D33" s="55"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="54"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="54"/>
     </row>
   </sheetData>
-  <mergeCells count="34">
+  <mergeCells count="40">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B3:D3"/>
@@ -3974,8 +4485,14 @@
     <mergeCell ref="B16:D16"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="G18:I18"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
   </mergeCells>
-  <conditionalFormatting sqref="M4 R4 R16 W4 W10 W16 AB10 AB16 AG4 AL4 AQ4 AV4 BA4 BF4 BK4 BP4">
+  <conditionalFormatting sqref="M4 C21 C26 R4 R16 W4:X4 W10 W16 AB16:AC16 AB10 AG4 AL4 AQ4 AV4 BA4 BF4 BK4 BP4">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Netzplan Übung 3 FIAE D Ressourcenübung
</commit_message>
<xml_diff>
--- a/FIAED Übungen/Online_Shop.Projekt.FIAE_D.xlsx
+++ b/FIAED Übungen/Online_Shop.Projekt.FIAE_D.xlsx
@@ -466,7 +466,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="58">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -647,6 +647,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -663,6 +667,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -687,7 +695,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -799,8 +807,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="5462280" y="479520"/>
-          <a:ext cx="5500800" cy="0"/>
+          <a:off x="5467680" y="479520"/>
+          <a:ext cx="5509440" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -841,7 +849,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5462640" y="488160"/>
+          <a:off x="5468040" y="488160"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -882,7 +890,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5461920" y="488160"/>
+          <a:off x="5467320" y="488160"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -924,7 +932,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5469840" y="1125360"/>
+          <a:off x="5475960" y="1125360"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -966,7 +974,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5469840" y="1612800"/>
+          <a:off x="5475960" y="1612800"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1008,7 +1016,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5469840" y="2099880"/>
+          <a:off x="5475960" y="2099880"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1050,7 +1058,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5469840" y="2587320"/>
+          <a:off x="5475960" y="2587320"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1092,7 +1100,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8210880" y="324720"/>
+          <a:off x="8221320" y="324720"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1134,7 +1142,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8210880" y="487440"/>
+          <a:off x="8221320" y="487440"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1176,7 +1184,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8210880" y="1125360"/>
+          <a:off x="8221320" y="1125360"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1218,7 +1226,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8210880" y="1612800"/>
+          <a:off x="8221320" y="1612800"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1260,7 +1268,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8210880" y="2587320"/>
+          <a:off x="8221320" y="2587320"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1302,7 +1310,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8210880" y="3074400"/>
+          <a:off x="8221320" y="3074400"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1344,7 +1352,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8210880" y="4048920"/>
+          <a:off x="8221320" y="4048920"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1386,7 +1394,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8210880" y="5023440"/>
+          <a:off x="8221320" y="5023440"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1428,7 +1436,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10952640" y="487440"/>
+          <a:off x="10966680" y="487440"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1470,7 +1478,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10952640" y="1125360"/>
+          <a:off x="10966680" y="1125360"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1512,7 +1520,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10952640" y="1612800"/>
+          <a:off x="10966680" y="1612800"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1554,7 +1562,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10952640" y="2099880"/>
+          <a:off x="10966680" y="2099880"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1596,7 +1604,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8208360" y="3557520"/>
+          <a:off x="8217360" y="3557520"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1638,7 +1646,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8208360" y="4533480"/>
+          <a:off x="8217360" y="4533480"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1680,7 +1688,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8208360" y="2093760"/>
+          <a:off x="8217360" y="2093760"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1710,15 +1718,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>10080</xdr:colOff>
+      <xdr:colOff>10440</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>154440</xdr:rowOff>
+      <xdr:rowOff>154800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>4680</xdr:colOff>
+      <xdr:colOff>5040</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>160560</xdr:rowOff>
+      <xdr:rowOff>160920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1727,7 +1735,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="7287120" y="479160"/>
+          <a:off x="9728280" y="479520"/>
           <a:ext cx="535680" cy="6120"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1752,15 +1760,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>268920</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>160560</xdr:rowOff>
+      <xdr:rowOff>160920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>268920</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>3600</xdr:rowOff>
+      <xdr:rowOff>3960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1769,7 +1777,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="8627040" y="485280"/>
+          <a:off x="11068560" y="485640"/>
           <a:ext cx="541080" cy="5400"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1794,15 +1802,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>255240</xdr:colOff>
+      <xdr:colOff>255600</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>18720</xdr:rowOff>
+      <xdr:rowOff>19440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>3600</xdr:colOff>
+      <xdr:colOff>3960</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>18720</xdr:rowOff>
+      <xdr:rowOff>19440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1811,7 +1819,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7532280" y="505800"/>
+          <a:off x="9973440" y="506520"/>
           <a:ext cx="18720" cy="1950840"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1836,15 +1844,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>12600</xdr:colOff>
+      <xdr:colOff>13320</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>159840</xdr:rowOff>
+      <xdr:rowOff>160200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>264960</xdr:colOff>
+      <xdr:colOff>265680</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>159840</xdr:rowOff>
+      <xdr:rowOff>160200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1853,7 +1861,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="7559640" y="2435400"/>
+          <a:off x="10001160" y="2435760"/>
           <a:ext cx="252360" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1878,15 +1886,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>5040</xdr:colOff>
+      <xdr:colOff>5400</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>154440</xdr:rowOff>
+      <xdr:rowOff>154800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>30</xdr:col>
       <xdr:colOff>244800</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>159840</xdr:rowOff>
+      <xdr:rowOff>160200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1895,7 +1903,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9987120" y="479160"/>
+          <a:off x="12428280" y="479520"/>
           <a:ext cx="1862640" cy="5400"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1920,15 +1928,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>268200</xdr:colOff>
+      <xdr:colOff>268560</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>160560</xdr:rowOff>
+      <xdr:rowOff>160920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>268200</xdr:colOff>
+      <xdr:colOff>268560</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>2880</xdr:rowOff>
+      <xdr:rowOff>3240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1937,7 +1945,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="8626680" y="2436120"/>
+          <a:off x="11068200" y="2436480"/>
           <a:ext cx="541080" cy="5040"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1964,13 +1972,13 @@
       <xdr:col>23</xdr:col>
       <xdr:colOff>266040</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>160560</xdr:rowOff>
+      <xdr:rowOff>160920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
       <xdr:colOff>260640</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>2880</xdr:rowOff>
+      <xdr:rowOff>3240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1979,7 +1987,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="9977400" y="2436120"/>
+          <a:off x="12418560" y="2436480"/>
           <a:ext cx="535680" cy="5040"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2004,15 +2012,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>257040</xdr:colOff>
+      <xdr:colOff>257400</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>158400</xdr:rowOff>
+      <xdr:rowOff>158760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>257040</xdr:colOff>
+      <xdr:colOff>257400</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>2880</xdr:rowOff>
+      <xdr:rowOff>3240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2021,7 +2029,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8886600" y="483120"/>
+          <a:off x="11327760" y="483480"/>
           <a:ext cx="0" cy="982440"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2046,15 +2054,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>253800</xdr:colOff>
+      <xdr:colOff>254520</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>155520</xdr:rowOff>
+      <xdr:rowOff>155880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>258840</xdr:colOff>
+      <xdr:colOff>259200</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>159480</xdr:rowOff>
+      <xdr:rowOff>159840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2063,7 +2071,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="8883000" y="1455480"/>
+          <a:off x="11324520" y="1455840"/>
           <a:ext cx="275400" cy="3960"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2094,7 +2102,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>12240</xdr:colOff>
+      <xdr:colOff>12600</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>162720</xdr:rowOff>
     </xdr:to>
@@ -2105,7 +2113,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9969480" y="1455840"/>
+          <a:off x="12410640" y="1455840"/>
           <a:ext cx="565920" cy="7200"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2147,7 +2155,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12677760" y="480240"/>
+          <a:off x="15118560" y="480240"/>
           <a:ext cx="560520" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2172,7 +2180,7 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>263880</xdr:colOff>
+      <xdr:colOff>264240</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>138600</xdr:rowOff>
     </xdr:from>
@@ -2189,7 +2197,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="10245960" y="1926720"/>
+          <a:off x="12687120" y="1926720"/>
           <a:ext cx="10080" cy="505440"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2214,15 +2222,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>264960</xdr:colOff>
+      <xdr:colOff>265680</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>155880</xdr:rowOff>
+      <xdr:rowOff>156240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
-      <xdr:colOff>257760</xdr:colOff>
+      <xdr:colOff>258480</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>160560</xdr:rowOff>
+      <xdr:rowOff>160920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2231,7 +2239,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="10246680" y="1943640"/>
+          <a:off x="12688200" y="1944000"/>
           <a:ext cx="1345320" cy="4680"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2256,15 +2264,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>29</xdr:col>
-      <xdr:colOff>263880</xdr:colOff>
+      <xdr:colOff>264600</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>146880</xdr:rowOff>
+      <xdr:rowOff>147240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
-      <xdr:colOff>264960</xdr:colOff>
+      <xdr:colOff>265680</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>25920</xdr:rowOff>
+      <xdr:rowOff>26280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2273,7 +2281,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="11598120" y="471600"/>
+          <a:off x="14039640" y="471960"/>
           <a:ext cx="1080" cy="1504440"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2298,7 +2306,7 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>29</xdr:col>
-      <xdr:colOff>1800</xdr:colOff>
+      <xdr:colOff>2160</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -2315,7 +2323,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11336400" y="1463040"/>
+          <a:off x="13777560" y="1463040"/>
           <a:ext cx="277920" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2340,13 +2348,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>39</xdr:col>
-      <xdr:colOff>10800</xdr:colOff>
+      <xdr:colOff>11160</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>153360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>41</xdr:col>
-      <xdr:colOff>29160</xdr:colOff>
+      <xdr:colOff>29520</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>153360</xdr:rowOff>
     </xdr:to>
@@ -2357,7 +2365,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14050440" y="478440"/>
+          <a:off x="16491600" y="478440"/>
           <a:ext cx="559440" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2388,7 +2396,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>46</xdr:col>
-      <xdr:colOff>18000</xdr:colOff>
+      <xdr:colOff>18360</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>156600</xdr:rowOff>
     </xdr:to>
@@ -2399,7 +2407,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15394680" y="478080"/>
+          <a:off x="17835840" y="478080"/>
           <a:ext cx="556560" cy="3600"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2424,15 +2432,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>49</xdr:col>
-      <xdr:colOff>21240</xdr:colOff>
+      <xdr:colOff>21600</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>160560</xdr:rowOff>
+      <xdr:rowOff>160920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>51</xdr:col>
-      <xdr:colOff>9720</xdr:colOff>
+      <xdr:colOff>10440</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>3600</xdr:rowOff>
+      <xdr:rowOff>3960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2441,7 +2449,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="16765560" y="485280"/>
+          <a:off x="19207080" y="485640"/>
           <a:ext cx="529560" cy="5400"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2466,15 +2474,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>53</xdr:col>
-      <xdr:colOff>251280</xdr:colOff>
+      <xdr:colOff>252000</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>155880</xdr:rowOff>
+      <xdr:rowOff>156240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>56</xdr:col>
-      <xdr:colOff>20520</xdr:colOff>
+      <xdr:colOff>20880</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>156960</xdr:rowOff>
+      <xdr:rowOff>157320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2483,7 +2491,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="18077760" y="480600"/>
+          <a:off x="20519280" y="480960"/>
           <a:ext cx="580680" cy="1080"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2508,15 +2516,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>58</xdr:col>
-      <xdr:colOff>252000</xdr:colOff>
+      <xdr:colOff>252360</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>156960</xdr:rowOff>
+      <xdr:rowOff>157320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>60</xdr:col>
-      <xdr:colOff>262440</xdr:colOff>
+      <xdr:colOff>262800</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>3600</xdr:rowOff>
+      <xdr:rowOff>3960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2525,7 +2533,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="19431360" y="481680"/>
+          <a:off x="21872520" y="482040"/>
           <a:ext cx="551520" cy="9000"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2550,15 +2558,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>64</xdr:col>
-      <xdr:colOff>1800</xdr:colOff>
+      <xdr:colOff>2160</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>156960</xdr:rowOff>
+      <xdr:rowOff>157320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>66</xdr:col>
       <xdr:colOff>2160</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>3600</xdr:rowOff>
+      <xdr:rowOff>3960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2567,7 +2575,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="20804040" y="481680"/>
+          <a:off x="23245200" y="482040"/>
           <a:ext cx="541080" cy="9000"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2592,15 +2600,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>64</xdr:col>
-      <xdr:colOff>263520</xdr:colOff>
+      <xdr:colOff>263880</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>3240</xdr:rowOff>
+      <xdr:rowOff>3600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>64</xdr:col>
-      <xdr:colOff>269640</xdr:colOff>
+      <xdr:colOff>270000</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>2880</xdr:rowOff>
+      <xdr:rowOff>3240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2609,7 +2617,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="21065760" y="490680"/>
+          <a:off x="23506920" y="491040"/>
           <a:ext cx="6120" cy="1950480"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2634,15 +2642,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>7920</xdr:colOff>
+      <xdr:colOff>8280</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>160560</xdr:rowOff>
+      <xdr:rowOff>160920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>259920</xdr:colOff>
+      <xdr:colOff>260280</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>4320</xdr:rowOff>
+      <xdr:rowOff>4680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2651,7 +2659,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="8637480" y="485280"/>
+          <a:off x="11078640" y="485640"/>
           <a:ext cx="252000" cy="6120"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2676,15 +2684,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>28</xdr:col>
-      <xdr:colOff>268920</xdr:colOff>
+      <xdr:colOff>269280</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>64</xdr:col>
-      <xdr:colOff>254520</xdr:colOff>
+      <xdr:colOff>254880</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>6120</xdr:rowOff>
+      <xdr:rowOff>6480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2693,7 +2701,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11332800" y="2437920"/>
+          <a:off x="13773960" y="2438280"/>
           <a:ext cx="9723960" cy="6120"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2725,11 +2733,11 @@
   </sheetPr>
   <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.96484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.77"/>
   </cols>
@@ -3272,20 +3280,18 @@
   </sheetPr>
   <dimension ref="A1:BQ35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="10" ySplit="0" topLeftCell="K10" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
-      <selection pane="topRight" activeCell="A32" activeCellId="0" sqref="A32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G24" activeCellId="0" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="20" width="11.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="16.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="8" min="7" style="3" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="9" min="9" style="21" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="8" min="7" style="3" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="9" min="9" style="21" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="3" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="107" min="11" style="0" width="3.83"/>
   </cols>
@@ -4275,7 +4281,7 @@
       <c r="H17" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="I17" s="35" t="n">
+      <c r="I17" s="45" t="n">
         <v>1</v>
       </c>
       <c r="J17" s="44" t="n">
@@ -4315,16 +4321,19 @@
       <c r="I18" s="31"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="45" t="s">
+      <c r="A19" s="46" t="s">
         <v>59</v>
       </c>
-      <c r="B19" s="46" t="s">
+      <c r="B19" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="C19" s="47"/>
-      <c r="D19" s="48" t="s">
+      <c r="C19" s="48"/>
+      <c r="D19" s="49" t="s">
         <v>61</v>
       </c>
+      <c r="G19" s="50"/>
+      <c r="H19" s="50"/>
+      <c r="I19" s="50"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="36" t="s">
@@ -4332,6 +4341,9 @@
       </c>
       <c r="C20" s="36"/>
       <c r="D20" s="36"/>
+      <c r="G20" s="50"/>
+      <c r="H20" s="50"/>
+      <c r="I20" s="50"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="36" t="s">
@@ -4343,21 +4355,27 @@
       <c r="D21" s="37" t="s">
         <v>63</v>
       </c>
+      <c r="G21" s="50"/>
+      <c r="H21" s="50"/>
+      <c r="I21" s="50"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="49" t="s">
+      <c r="A22" s="51" t="s">
         <v>64</v>
       </c>
-      <c r="B22" s="50" t="s">
+      <c r="B22" s="52" t="s">
         <v>60</v>
       </c>
-      <c r="C22" s="51"/>
-      <c r="D22" s="52" t="s">
+      <c r="C22" s="53"/>
+      <c r="D22" s="54" t="s">
         <v>61</v>
       </c>
+      <c r="G22" s="50"/>
+      <c r="H22" s="50"/>
+      <c r="I22" s="50"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="53" t="s">
+      <c r="B24" s="55" t="s">
         <v>65</v>
       </c>
       <c r="C24" s="31"/>
@@ -4384,7 +4402,7 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="53" t="s">
+      <c r="B27" s="55" t="s">
         <v>71</v>
       </c>
       <c r="C27" s="31"/>
@@ -4396,61 +4414,61 @@
       <c r="A29" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="B29" s="54" t="s">
+      <c r="B29" s="56" t="s">
         <v>73</v>
       </c>
-      <c r="C29" s="55" t="s">
+      <c r="C29" s="57" t="s">
         <v>74</v>
       </c>
-      <c r="D29" s="55"/>
+      <c r="D29" s="57"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="B30" s="54" t="s">
+      <c r="B30" s="56" t="s">
         <v>73</v>
       </c>
-      <c r="C30" s="55" t="s">
+      <c r="C30" s="57" t="s">
         <v>75</v>
       </c>
-      <c r="D30" s="55"/>
+      <c r="D30" s="57"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="54"/>
+      <c r="B31" s="56"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="B32" s="54" t="s">
+      <c r="B32" s="56" t="s">
         <v>73</v>
       </c>
-      <c r="C32" s="55" t="s">
+      <c r="C32" s="57" t="s">
         <v>75</v>
       </c>
-      <c r="D32" s="55"/>
+      <c r="D32" s="57"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="B33" s="54" t="s">
+      <c r="B33" s="56" t="s">
         <v>73</v>
       </c>
-      <c r="C33" s="55" t="s">
+      <c r="C33" s="57" t="s">
         <v>74</v>
       </c>
-      <c r="D33" s="55"/>
+      <c r="D33" s="57"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="54"/>
+      <c r="B34" s="56"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="54"/>
+      <c r="B35" s="56"/>
     </row>
   </sheetData>
-  <mergeCells count="40">
+  <mergeCells count="41">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B3:D3"/>
@@ -4485,6 +4503,7 @@
     <mergeCell ref="B16:D16"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="G18:I18"/>
+    <mergeCell ref="G19:I22"/>
     <mergeCell ref="B20:D20"/>
     <mergeCell ref="B25:D25"/>
     <mergeCell ref="C29:D29"/>

</xml_diff>

<commit_message>
Ressourcenplanung Online Shop Projekt
</commit_message>
<xml_diff>
--- a/FIAED Übungen/Online_Shop.Projekt.FIAE_D.xlsx
+++ b/FIAED Übungen/Online_Shop.Projekt.FIAE_D.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PSP" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="77">
   <si>
     <t xml:space="preserve">Beispiel: Funktionsorientierter Projektstrukturplan</t>
   </si>
@@ -187,6 +187,9 @@
   </si>
   <si>
     <t xml:space="preserve">1.1.2, 1.1.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2</t>
   </si>
   <si>
     <t xml:space="preserve">1.2.4, 1.3.1</t>
@@ -2733,7 +2736,7 @@
   </sheetPr>
   <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -3280,8 +3283,8 @@
   </sheetPr>
   <dimension ref="A1:BQ35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G24" activeCellId="0" sqref="G24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
@@ -3355,6 +3358,7 @@
       </c>
       <c r="M2" s="31"/>
       <c r="N2" s="30" t="n">
+        <f aca="false">L2+L4</f>
         <v>5</v>
       </c>
       <c r="Q2" s="30" t="n">
@@ -3362,84 +3366,89 @@
       </c>
       <c r="R2" s="31"/>
       <c r="S2" s="30" t="n">
+        <f aca="false">Q2+Q4</f>
         <v>6</v>
       </c>
       <c r="V2" s="30" t="n">
+        <f aca="false">S2</f>
         <v>6</v>
       </c>
       <c r="W2" s="31"/>
       <c r="X2" s="30" t="n">
+        <f aca="false">V2+V4</f>
         <v>10</v>
       </c>
       <c r="AF2" s="30" t="n">
-        <v>16</v>
+        <f aca="false">MAX(X2,AC8,X14)</f>
+        <v>14</v>
       </c>
       <c r="AG2" s="31"/>
       <c r="AH2" s="30" t="n">
-        <v>18</v>
+        <f aca="false">AF2+AF4</f>
+        <v>15</v>
       </c>
       <c r="AK2" s="30" t="n">
         <f aca="false">AH2</f>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="AL2" s="31"/>
       <c r="AM2" s="30" t="n">
         <f aca="false">AK2+AK4</f>
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="AP2" s="30" t="n">
         <f aca="false">AM2</f>
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="AQ2" s="31"/>
       <c r="AR2" s="30" t="n">
         <f aca="false">AP2+AP4</f>
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="AU2" s="30" t="n">
         <f aca="false">AR2</f>
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="AV2" s="31"/>
       <c r="AW2" s="30" t="n">
         <f aca="false">AU2+AU4</f>
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AZ2" s="30" t="n">
         <f aca="false">AW2</f>
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="BA2" s="31"/>
       <c r="BB2" s="30" t="n">
         <f aca="false">AZ2+AZ4</f>
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="BE2" s="30" t="n">
         <f aca="false">BB2</f>
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="BF2" s="31"/>
       <c r="BG2" s="30" t="n">
         <f aca="false">BE2+BE4</f>
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="BJ2" s="30" t="n">
         <f aca="false">BG2</f>
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="BK2" s="31"/>
       <c r="BL2" s="30" t="n">
         <f aca="false">BJ2+BJ4</f>
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="BO2" s="30" t="n">
         <f aca="false">MAX(BL2,AC14)</f>
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="BP2" s="31"/>
       <c r="BQ2" s="30" t="n">
         <f aca="false">BO2+BO4</f>
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3572,7 +3581,7 @@
       </c>
       <c r="R4" s="38" t="n">
         <f aca="false">S5-S2</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="S4" s="37" t="n">
         <f aca="false">MIN(V2,V8)-S2</f>
@@ -3584,19 +3593,19 @@
       </c>
       <c r="W4" s="38" t="n">
         <f aca="false">X5-X2</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="X4" s="38" t="n">
         <f aca="false">AF2-X2</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="AF4" s="37" t="n">
         <f aca="false">VLOOKUP(AF3,$A$2:$J$17,10)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AG4" s="38" t="n">
         <f aca="false">AH5-AH2</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AH4" s="37" t="n">
         <f aca="false">AK2-AH2</f>
@@ -3604,11 +3613,11 @@
       </c>
       <c r="AK4" s="37" t="n">
         <f aca="false">VLOOKUP(AK3,$A$2:$J$17,10)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AL4" s="38" t="n">
         <f aca="false">AM5-AM2</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AM4" s="37" t="n">
         <f aca="false">AP2-AM2</f>
@@ -3616,11 +3625,11 @@
       </c>
       <c r="AP4" s="37" t="n">
         <f aca="false">VLOOKUP(AP3,$A$2:$J$17,10)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AQ4" s="38" t="n">
         <f aca="false">AR5-AR2</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AR4" s="37" t="n">
         <f aca="false">AU2-AR2</f>
@@ -3632,19 +3641,19 @@
       </c>
       <c r="AV4" s="38" t="n">
         <f aca="false">AW5-AW2</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AW4" s="37" t="n">
         <f aca="false">AZ2-AW2</f>
         <v>0</v>
       </c>
       <c r="AZ4" s="37" t="n">
-        <f aca="false">VLOOKUP(AZ3,$A$2:$J$17,10)</f>
+        <f aca="false">J14</f>
         <v>2</v>
       </c>
       <c r="BA4" s="38" t="n">
         <f aca="false">BB5-BB2</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BB4" s="37" t="n">
         <f aca="false">BE2-BB2</f>
@@ -3656,7 +3665,7 @@
       </c>
       <c r="BF4" s="38" t="n">
         <f aca="false">BG5-BG2</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BG4" s="37" t="n">
         <f aca="false">BJ2-BG2</f>
@@ -3667,11 +3676,11 @@
       </c>
       <c r="BK4" s="38" t="n">
         <f aca="false">BL5-BL2</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BL4" s="37" t="n">
         <f aca="false">BO2-BL2</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BO4" s="37" t="n">
         <v>1</v>
@@ -3720,24 +3729,25 @@
       </c>
       <c r="Q5" s="30" t="n">
         <f aca="false">S5-Q4</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="R5" s="31"/>
       <c r="S5" s="30" t="n">
         <f aca="false">MIN(V5,V11)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="V5" s="30" t="n">
         <f aca="false">X5-V4</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="W5" s="31"/>
       <c r="X5" s="30" t="n">
-        <v>16</v>
+        <f aca="false">AF5</f>
+        <v>17</v>
       </c>
       <c r="AF5" s="30" t="n">
         <f aca="false">AH5-AF4</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AG5" s="31"/>
       <c r="AH5" s="30" t="n">
@@ -3751,60 +3761,61 @@
       <c r="AL5" s="31"/>
       <c r="AM5" s="30" t="n">
         <f aca="false">AP5</f>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="AP5" s="30" t="n">
         <f aca="false">AR5-AP4</f>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="AQ5" s="31"/>
       <c r="AR5" s="30" t="n">
         <f aca="false">AU5</f>
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="AU5" s="30" t="n">
         <f aca="false">AW5-AU4</f>
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="AV5" s="31"/>
       <c r="AW5" s="30" t="n">
         <f aca="false">AZ5</f>
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="AZ5" s="30" t="n">
         <f aca="false">BB5-AZ4</f>
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="BA5" s="31"/>
       <c r="BB5" s="30" t="n">
         <f aca="false">BE5</f>
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="BE5" s="30" t="n">
         <f aca="false">BG5-BE4</f>
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="BF5" s="31"/>
       <c r="BG5" s="30" t="n">
         <f aca="false">BJ5</f>
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="BJ5" s="30" t="n">
         <f aca="false">BL5-BJ4</f>
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="BK5" s="31"/>
       <c r="BL5" s="30" t="n">
-        <v>33</v>
+        <f aca="false">BO5</f>
+        <v>31</v>
       </c>
       <c r="BO5" s="30" t="n">
         <f aca="false">BQ5-BO4</f>
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="BP5" s="31"/>
       <c r="BQ5" s="30" t="n">
         <f aca="false">BQ2</f>
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3826,14 +3837,15 @@
         <v>7</v>
       </c>
       <c r="H6" s="33" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="I6" s="35" t="n">
-        <v>1</v>
+        <f aca="false">(100%+(100%-$I$12))/H6</f>
+        <v>0.775</v>
       </c>
       <c r="J6" s="34" t="n">
         <f aca="false">ROUND(G6/(H6*I6),0)</f>
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3878,7 +3890,7 @@
         <v>22</v>
       </c>
       <c r="F8" s="39" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G8" s="40" t="n">
         <v>3</v>
@@ -3898,14 +3910,17 @@
       </c>
       <c r="W8" s="31"/>
       <c r="X8" s="30" t="n">
+        <f aca="false">V8+V10</f>
         <v>9</v>
       </c>
       <c r="AA8" s="30" t="n">
+        <f aca="false">X8</f>
         <v>9</v>
       </c>
       <c r="AB8" s="31"/>
       <c r="AC8" s="30" t="n">
-        <v>16</v>
+        <f aca="false">AA8+AA10</f>
+        <v>14</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3918,7 +3933,7 @@
       <c r="C9" s="32"/>
       <c r="D9" s="32"/>
       <c r="E9" s="39" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F9" s="39" t="s">
         <v>35</v>
@@ -3927,14 +3942,15 @@
         <v>2</v>
       </c>
       <c r="H9" s="33" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="I9" s="35" t="n">
-        <v>1</v>
+        <f aca="false">(100%+(100%-$I$12))/H9</f>
+        <v>0.775</v>
       </c>
       <c r="J9" s="34" t="n">
         <f aca="false">ROUND(G9/(H9*I9),0)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V9" s="36" t="s">
         <v>27</v>
@@ -3966,14 +3982,15 @@
         <v>2</v>
       </c>
       <c r="H10" s="33" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="I10" s="35" t="n">
-        <v>1</v>
+        <f aca="false">(100%+(100%-$I$12))/H10</f>
+        <v>0.775</v>
       </c>
       <c r="J10" s="34" t="n">
         <f aca="false">ROUND(G10/(H10*I10),0)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V10" s="37" t="n">
         <f aca="false">VLOOKUP(V9,$A$2:$J$17,10)</f>
@@ -3981,7 +3998,7 @@
       </c>
       <c r="W10" s="38" t="n">
         <f aca="false">X11-X8</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="X10" s="37" t="n">
         <f aca="false">AA8-X8</f>
@@ -3989,11 +4006,11 @@
       </c>
       <c r="AA10" s="37" t="n">
         <f aca="false">VLOOKUP(AA9,$A$2:$J$17,10)</f>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="AB10" s="38" t="n">
         <f aca="false">AC11-AC8</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AC10" s="37" t="n">
         <f aca="false">AF2-AC8</f>
@@ -4019,30 +4036,33 @@
         <v>2</v>
       </c>
       <c r="H11" s="33" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="I11" s="35" t="n">
-        <v>1</v>
+        <f aca="false">(100%+(100%-$I$12))/H11</f>
+        <v>0.775</v>
       </c>
       <c r="J11" s="34" t="n">
         <f aca="false">ROUND(G11/(H11*I11),0)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V11" s="30" t="n">
         <f aca="false">X11-V10</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="W11" s="31"/>
       <c r="X11" s="30" t="n">
-        <v>9</v>
+        <f aca="false">AA11</f>
+        <v>12</v>
       </c>
       <c r="AA11" s="30" t="n">
         <f aca="false">AC11-AA10</f>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="AB11" s="31"/>
       <c r="AC11" s="30" t="n">
-        <v>16</v>
+        <f aca="false">AF5</f>
+        <v>17</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4050,7 +4070,7 @@
         <v>17</v>
       </c>
       <c r="B12" s="32" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C12" s="32"/>
       <c r="D12" s="32"/>
@@ -4067,11 +4087,11 @@
         <v>53</v>
       </c>
       <c r="I12" s="35" t="n">
-        <v>1</v>
+        <v>0.45</v>
       </c>
       <c r="J12" s="34" t="n">
         <f aca="false">ROUND(G12/(H12*I12),0)</f>
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4122,35 +4142,42 @@
         <v>3</v>
       </c>
       <c r="H14" s="33" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="I14" s="35" t="n">
-        <v>1</v>
+        <f aca="false">(100%+(100%-$I$12))/H14</f>
+        <v>0.775</v>
       </c>
       <c r="J14" s="34" t="n">
         <f aca="false">ROUND(G14/(H14*I14),0)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q14" s="30" t="n">
+        <f aca="false">N2</f>
         <v>5</v>
       </c>
       <c r="R14" s="31"/>
       <c r="S14" s="30" t="n">
+        <f aca="false">Q14+Q16</f>
         <v>6</v>
       </c>
       <c r="V14" s="30" t="n">
+        <f aca="false">S14</f>
         <v>6</v>
       </c>
       <c r="W14" s="31"/>
       <c r="X14" s="30" t="n">
+        <f aca="false">V14+V16</f>
         <v>9</v>
       </c>
       <c r="AA14" s="30" t="n">
+        <f aca="false">X14</f>
         <v>9</v>
       </c>
       <c r="AB14" s="31"/>
       <c r="AC14" s="30" t="n">
-        <v>19</v>
+        <f aca="false">AA14+AA16</f>
+        <v>31</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4216,14 +4243,15 @@
         <v>5</v>
       </c>
       <c r="H16" s="33" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="I16" s="35" t="n">
-        <v>1</v>
+        <f aca="false">(100%+(100%-$I$12))/H16</f>
+        <v>0.775</v>
       </c>
       <c r="J16" s="34" t="n">
         <f aca="false">ROUND(G16/(H16*I16),0)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="Q16" s="37" t="n">
         <f aca="false">VLOOKUP(Q15,$A$2:$J$17,10)</f>
@@ -4231,7 +4259,7 @@
       </c>
       <c r="R16" s="38" t="n">
         <f aca="false">S17-S14</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="S16" s="37" t="n">
         <f aca="false">V14-S14</f>
@@ -4243,7 +4271,7 @@
       </c>
       <c r="W16" s="38" t="n">
         <f aca="false">X17-X14</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="X16" s="37" t="n">
         <f aca="false">MIN(AA14,AF2)-X14</f>
@@ -4251,15 +4279,15 @@
       </c>
       <c r="AA16" s="37" t="n">
         <f aca="false">VLOOKUP(AA15,$A$2:$J$17,10)</f>
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="AB16" s="38" t="n">
         <f aca="false">AC17-AC14</f>
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="AC16" s="38" t="n">
         <f aca="false">BO2-AC14</f>
-        <v>14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4272,7 +4300,7 @@
       <c r="C17" s="41"/>
       <c r="D17" s="41"/>
       <c r="E17" s="42" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F17" s="43"/>
       <c r="G17" s="44" t="n">
@@ -4290,29 +4318,30 @@
       </c>
       <c r="Q17" s="30" t="n">
         <f aca="false">S17-Q16</f>
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="R17" s="31"/>
       <c r="S17" s="30" t="n">
         <f aca="false">V17</f>
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="V17" s="30" t="n">
         <f aca="false">X17-V16</f>
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="W17" s="31"/>
       <c r="X17" s="30" t="n">
-        <f aca="false">MIN(AF5,AA17)</f>
-        <v>16</v>
+        <f aca="false">MIN(AA17,AF5)</f>
+        <v>9</v>
       </c>
       <c r="AA17" s="30" t="n">
         <f aca="false">AC17-AA16</f>
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="AB17" s="31"/>
       <c r="AC17" s="30" t="n">
-        <v>33</v>
+        <f aca="false">BO5</f>
+        <v>31</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4322,14 +4351,14 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="46" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B19" s="47" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C19" s="48"/>
       <c r="D19" s="49" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G19" s="50"/>
       <c r="H19" s="50"/>
@@ -4350,10 +4379,10 @@
         <v>51</v>
       </c>
       <c r="C21" s="38" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D21" s="37" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G21" s="50"/>
       <c r="H21" s="50"/>
@@ -4361,14 +4390,14 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="51" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B22" s="52" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C22" s="53"/>
       <c r="D22" s="54" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G22" s="50"/>
       <c r="H22" s="50"/>
@@ -4376,61 +4405,61 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="55" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C24" s="31"/>
       <c r="D24" s="30" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="36" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C25" s="36"/>
       <c r="D25" s="36"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="36" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C26" s="38" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D26" s="37" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="55" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C27" s="31"/>
       <c r="D27" s="30" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B29" s="56" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C29" s="57" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D29" s="57"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B30" s="56" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C30" s="57" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D30" s="57"/>
     </row>
@@ -4439,25 +4468,25 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B32" s="56" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C32" s="57" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D32" s="57"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B33" s="56" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C33" s="57" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D33" s="57"/>
     </row>

</xml_diff>